<commit_message>
updated BOM for sprite DevBoard replica
</commit_message>
<xml_diff>
--- a/sprite/DevBoard_Files/BOM.xlsx
+++ b/sprite/DevBoard_Files/BOM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hall\Desktop\PCBSat\sprite\DevBoard_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BDFE6C30-2AF0-4A4A-9724-76277B0052D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7110" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,8 +28,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="BOM" type="6" refreshedVersion="0" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="BOM" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="9" sourceFile="Macintosh HD:Users:zacman:Documents:GitHub:kicksat:Sprite:EagleCAD:Sprite:DevBoard_Files:BOM" space="1" consecutive="1">
       <textFields count="6">
         <textField type="text"/>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="132">
   <si>
     <t>Part</t>
   </si>
@@ -233,9 +239,6 @@
     <t>QFN-48</t>
   </si>
   <si>
-    <t>16-LPCC</t>
-  </si>
-  <si>
     <t>DNP</t>
   </si>
   <si>
@@ -305,9 +308,6 @@
     <t>296-27420-1-ND</t>
   </si>
   <si>
-    <t>342-1082-1-ND</t>
-  </si>
-  <si>
     <t>535-9815-1-ND</t>
   </si>
   <si>
@@ -362,20 +362,92 @@
     <t>CC430F5137IRGZR</t>
   </si>
   <si>
-    <t>HMC5883L-TR</t>
-  </si>
-  <si>
     <t>ABM11-26.000MHZ-B7G-T</t>
   </si>
   <si>
     <t>C0603C222K5RACTU</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Desicription</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>Chip LED</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>Triangular Advanced Solar Cell</t>
+  </si>
+  <si>
+    <t>MSP430 w/ Integrated Radio</t>
+  </si>
+  <si>
+    <t>3-Axis Digital Compass</t>
+  </si>
+  <si>
+    <t>3-Axis Gyroscope</t>
+  </si>
+  <si>
+    <t>Quartz Crystal</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/invensense/itg-3200/gyroscope-mems-triple-axis-qfn/dp/37T8091?ost=37T8091&amp;ddkey=http%3Aen-US%2FElement14_US%2Fsearch#anchorTechnicalDOCS</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Ferrite Rod</t>
+  </si>
+  <si>
+    <t>623-4052077111 (Mouser)</t>
+  </si>
+  <si>
+    <t>Fair-Rite Ferrite Rod</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Fair-Rite/4052077111?qs=%2fha2pyFaduiKM3OCAU9mDEWvBx05GYrQFGX1acsL9DE%3d</t>
+  </si>
+  <si>
+    <t>1267-1072-1-ND</t>
+  </si>
+  <si>
+    <t>16-LGA</t>
+  </si>
+  <si>
+    <t>MMC5883MA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/memsic-inc/MMC5883MA/1267-1072-1-ND/7063085</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=296-27420-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=535-9815-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -428,6 +500,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -467,7 +551,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -483,6 +567,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -501,11 +590,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="BOM" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -829,24 +926,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.625" customWidth="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -860,13 +958,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>71</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -879,14 +986,17 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -899,14 +1009,17 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -919,14 +1032,17 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -939,14 +1055,17 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -959,14 +1078,17 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -979,14 +1101,17 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -999,14 +1124,17 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1019,14 +1147,17 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1039,14 +1170,17 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1059,14 +1193,17 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1079,14 +1216,17 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1099,14 +1239,17 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1119,14 +1262,17 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1139,14 +1285,17 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1159,14 +1308,17 @@
       <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="E16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1179,14 +1331,17 @@
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="E17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1199,14 +1354,17 @@
       <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1219,14 +1377,17 @@
       <c r="D19" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="E19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1239,14 +1400,17 @@
       <c r="D20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="E20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -1259,54 +1423,63 @@
       <c r="D21" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
+      <c r="G22" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
         <v>66</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C23" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D23" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="E23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1319,16 +1492,19 @@
       <c r="D24" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="E24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
         <v>46</v>
@@ -1339,14 +1515,17 @@
       <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1359,14 +1538,23 @@
       <c r="D26" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>87</v>
+      <c r="E26" t="s">
+        <v>114</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>86</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26">
+        <v>6.59</v>
+      </c>
+      <c r="I26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1374,19 +1562,28 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="E27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27">
+        <v>5.47</v>
+      </c>
+      <c r="I27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1400,13 +1597,22 @@
         <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="H28">
+        <v>14.45</v>
+      </c>
+      <c r="I28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -1420,80 +1626,126 @@
         <v>56</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>117</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29">
+        <v>1.68</v>
+      </c>
+      <c r="I29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="12">
+        <v>4052077111</v>
+      </c>
+      <c r="H30">
+        <v>0.16</v>
+      </c>
+      <c r="I30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>